<commit_message>
Adding task order specification to be able to distinguish between tasks with the same number of volumes and sequence name (order specified in tha datasheet).
</commit_message>
<xml_diff>
--- a/code/RaBIDS templates/datasheet.xlsx
+++ b/code/RaBIDS templates/datasheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\_RaBIDS\clone github repository\RaBIDS\code\RaBIDS templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\zisvfs12\Home\miroslava.jindrova\Documents\repos\RaBIDS\code\RaBIDS templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28520" windowHeight="12590"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28524" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="datasheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
   <si>
     <t>SPM</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>TaskOrder</t>
+  </si>
+  <si>
+    <t>Defining the order of the sequences with the same series ID and overlapping number of volumes</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -278,10 +287,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -586,22 +596,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -618,10 +628,13 @@
         <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -637,11 +650,11 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -657,11 +670,11 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -678,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -695,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -711,11 +724,11 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -731,11 +744,11 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -751,11 +764,11 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -765,14 +778,14 @@
       <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -783,7 +796,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -794,7 +807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -810,11 +823,11 @@
       <c r="E15" t="s">
         <v>63</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -824,8 +837,14 @@
       <c r="C16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -838,11 +857,11 @@
       <c r="D17" t="s">
         <v>63</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -853,7 +872,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -867,7 +886,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -878,7 +897,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -891,11 +910,11 @@
       <c r="D21" t="s">
         <v>63</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -911,11 +930,11 @@
       <c r="E22" t="s">
         <v>63</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -925,11 +944,11 @@
       <c r="C24" t="s">
         <v>66</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -939,11 +958,11 @@
       <c r="C26" t="s">
         <v>65</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -951,7 +970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -965,7 +984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -976,7 +995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -987,7 +1006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>24</v>
       </c>

</xml_diff>